<commit_message>
v3.0.2 clean thr code
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\citylink\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\citylinktech\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="11" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3328" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3328" uniqueCount="572">
   <si>
     <t>Date</t>
   </si>
@@ -1738,6 +1738,12 @@
   </si>
   <si>
     <t>Inactive</t>
+  </si>
+  <si>
+    <t>Not Satisfied</t>
+  </si>
+  <si>
+    <t>In Active</t>
   </si>
 </sst>
 </file>
@@ -2108,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="A20:E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2417,7 +2423,7 @@
   <dimension ref="A1:U261"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2489,10 +2495,10 @@
         <v>45298</v>
       </c>
       <c r="G2" s="13">
-        <v>0.70833333333333304</v>
+        <v>1.2083333333333299</v>
       </c>
       <c r="H2" s="13">
-        <v>0.70833333333333304</v>
+        <v>1.4583333333333299</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>542</v>
@@ -2532,10 +2538,10 @@
         <v>45306</v>
       </c>
       <c r="G3" s="13">
-        <v>0.70833333333333304</v>
+        <v>1.2083333333333299</v>
       </c>
       <c r="H3" s="13">
-        <v>0.70833333333333304</v>
+        <v>1.4583333333333299</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>542</v>
@@ -2578,7 +2584,7 @@
         <v>1.2083333333333299</v>
       </c>
       <c r="H4" s="13">
-        <v>1.2083333333333299</v>
+        <v>1.4583333333333299</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>542</v>
@@ -2618,10 +2624,10 @@
         <v>45327</v>
       </c>
       <c r="G5" s="13">
-        <v>0.70833333333333304</v>
+        <v>1.25</v>
       </c>
       <c r="H5" s="13">
-        <v>0.70833333333333304</v>
+        <v>1.2916666666666701</v>
       </c>
       <c r="I5" s="11" t="s">
         <v>542</v>
@@ -2661,10 +2667,10 @@
         <v>45334</v>
       </c>
       <c r="G6" s="13">
-        <v>1.2083333333333299</v>
+        <v>1.2916666666666601</v>
       </c>
       <c r="H6" s="13">
-        <v>1.2083333333333299</v>
+        <v>1.3333333333333299</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>542</v>
@@ -2704,10 +2710,10 @@
         <v>45340</v>
       </c>
       <c r="G7" s="13">
-        <v>0.95833333333333304</v>
+        <v>1.3333333333333299</v>
       </c>
       <c r="H7" s="13">
-        <v>0.95833333333333304</v>
+        <v>1.375</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>542</v>
@@ -2747,10 +2753,10 @@
         <v>45349</v>
       </c>
       <c r="G8" s="13">
-        <v>0.95833333333333304</v>
+        <v>1.375</v>
       </c>
       <c r="H8" s="13">
-        <v>0.95833333333333304</v>
+        <v>1.4166666666666701</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>546</v>
@@ -2793,7 +2799,7 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="H9" s="13">
-        <v>0.95833333333333304</v>
+        <v>1</v>
       </c>
       <c r="I9" s="11" t="s">
         <v>542</v>
@@ -2836,13 +2842,13 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="H10" s="13">
-        <v>0.95833333333333304</v>
+        <v>1</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>546</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -2879,7 +2885,7 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="H11" s="13">
-        <v>0.70833333333333304</v>
+        <v>0.75</v>
       </c>
       <c r="I11" s="11" t="s">
         <v>542</v>
@@ -3874,7 +3880,7 @@
         <v>542</v>
       </c>
       <c r="J34" s="11" t="s">
-        <v>544</v>
+        <v>564</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -8210,8 +8216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L262"/>
   <sheetViews>
-    <sheetView topLeftCell="A256" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B262" sqref="B262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8294,7 +8300,7 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="I2" s="14">
-        <v>0.95833333333333304</v>
+        <v>0.5</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>4</v>
@@ -8332,7 +8338,7 @@
         <v>1.2083333333333299</v>
       </c>
       <c r="I3" s="14">
-        <v>1.2083333333333299</v>
+        <v>1.25</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>4</v>
@@ -8370,7 +8376,7 @@
         <v>1.4583333333333299</v>
       </c>
       <c r="I4" s="14">
-        <v>1.4583333333333299</v>
+        <v>1</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>4</v>
@@ -8408,7 +8414,7 @@
         <v>1.7083333333333299</v>
       </c>
       <c r="I5" s="14">
-        <v>1.7083333333333299</v>
+        <v>1.8333333333333299</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>4</v>
@@ -8446,7 +8452,7 @@
         <v>1.9583333333333299</v>
       </c>
       <c r="I6" s="14">
-        <v>1.9583333333333299</v>
+        <v>1.5</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>4</v>
@@ -8484,7 +8490,7 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="I7" s="14">
-        <v>0.70833333333333304</v>
+        <v>0.875</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>4</v>
@@ -8522,7 +8528,7 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="I8" s="14">
-        <v>0.95833333333333304</v>
+        <v>0.5</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>4</v>
@@ -8560,7 +8566,7 @@
         <v>1.2083333333333299</v>
       </c>
       <c r="I9" s="14">
-        <v>1.2083333333333299</v>
+        <v>1.4583333333333299</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>4</v>
@@ -16125,7 +16131,7 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="J208" s="10" t="s">
-        <v>4</v>
+        <v>571</v>
       </c>
       <c r="K208" s="10">
         <v>4.5</v>

</xml_diff>